<commit_message>
refactored rag llm eval
</commit_message>
<xml_diff>
--- a/resources/TestData/LLM_evaluator_dataset.xlsx
+++ b/resources/TestData/LLM_evaluator_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VM116ZZ\PycharmProjects\POC\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6263C9B-364C-4190-9D4A-EB1087C8500B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309724B9-9708-47CD-8690-B60771C1E114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5CCB64F4-7660-471E-B1F7-FBD933439687}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>question</t>
   </si>
@@ -234,6 +234,24 @@
   </si>
   <si>
     <t>You fool I am not here to answer stupid questions.</t>
+  </si>
+  <si>
+    <t>Can lambdas return a value ?</t>
+  </si>
+  <si>
+    <t>Is selenium used for automation testing ?</t>
+  </si>
+  <si>
+    <t>Lambdas may return a value. The type of the return value will be inferred by compiler. The return statement is not required if the lambda body is just a one-liner. The two code snippets below are equivalent: Arrays.asList( 'a', 'b', 'd' ).sort( ( e1, e2 ) -&gt; e1.compareTo( e2 ) ); And: Arrays.asList( 'a', 'b'', 'd'' ).sort( ( e1, e2 ) -&gt; { int result = e1.compareTo( e2 ); return result; } ); to new concise and compact language constructs. In its simplest form, a lambda could be represented as a comma-separated list of parameters, the →symbol and the body. For example: Arrays.asList( 'a'', 'b', 'd' ).forEach( e -&gt; System.out.println( e ) ); Please notice the type of argument e is being inferred by the compiler. Alternatively, you may explicitly provide the type of the parameter, wrapping the deﬁnition in brackets. For example: it does not even use the word lambda. In Java, the lambda expre ssion for a squaring function like the one above can be written x -&gt; x*x The operator -&gt; is what makes this a lambda expression. The dummy parameter f or the function is on the left of the operator, and the expression that comput es the value of the function is on the right.</t>
+  </si>
+  <si>
+    <t>Selenium is widely used for automation testing of web applications.Selenium is an open-source framework that allows you to automate web browser actions, such as clicking buttons, filling forms, and verifying content.</t>
+  </si>
+  <si>
+    <t>Lambdas may return a value. The type of the return value will be inferred by compiler. The return statement is not required if the lambda body is just a one-liner. The two code snippets below are equivalent: Arrays.asList( 'a', 'b', 'd' ).sort( ( e1, e2 ) -&gt; e1.compareTo( e2 ) ); And: Arrays.asList( 'a', 'b'', 'd'' ).sort( ( e1, e2 ) -&gt; { int result = e1.compareTo( e2 ); return result; } ); to new concise and compact language constructs. In its simplest form, a lambda could be represented as a comma-separated list of parameters, the →symbol and the body. For example: Arrays.asList( 'a'', 'b', 'd' ).forEach( e -&gt; System.out.println( e ) ); Please notice the type of argument e is being inferred by the compiler. Alternatively, you may explicitly provide the type of the parameter, wrapping the deﬁnition in brackets. For example: it does not even use the word lambda. In Java, the lambda expre ssion for a squaring function like the one above can be written x -&gt; x*x The operator -&gt; is what makes this a lambda expression. The dummy parameter f or the function is on the left of the operator</t>
+  </si>
+  <si>
+    <t>INTRODUCTION OF AUTOMATION TESTING Important Java concepts required for selenium Conditions if if else switch Loops for while do while for each Oops Inheritance Polymorphism Encapsulation Abstraction Method overloading overriding Constructors String Type casting Upcasting Code optimization Collection List and Set Automation Performing any task by using a tool or machine is called as automation Advantages 1 Save the time 2 Faster Selenium Its a free and open source automation tool which is used to automation any web based applications Advantages of selenium It is freely available automation tool To make use of selenium for commercial purpose we dont have to buy any license It is available in below website httpswwwseleniumhqorgdownload Anyone can view source code of selenium which is available in below website httpsgithubcomSeleniumHQselenium Automation Tool Its a software or an application which is used to automate any applications Ex Selenium QTP Appium AutoIT etc</t>
   </si>
 </sst>
 </file>
@@ -619,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B03D3C5-413B-466A-9768-11DD34F79034}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -869,6 +887,28 @@
         <v>61</v>
       </c>
     </row>
+    <row r="23" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>